<commit_message>
change object name `table_definition` to `columns` .
</commit_message>
<xml_diff>
--- a/tests/testdata/db/sample_db_tables.xlsx
+++ b/tests/testdata/db/sample_db_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="table_user" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">user</t>
   </si>
   <si>
-    <t xml:space="preserve">:column_definition</t>
+    <t xml:space="preserve">:columns</t>
   </si>
   <si>
     <t xml:space="preserve">column_name</t>
@@ -180,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Hiragino Mincho ProN"/>
@@ -252,6 +252,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -268,6 +269,12 @@
       <sz val="10"/>
       <color rgb="FFB2B2B2"/>
       <name val="Hiragino Mincho ProN"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -432,7 +439,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -441,6 +448,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,11 +460,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,8 +567,8 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,331 +590,331 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="5"/>
+      <c r="F8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -919,7 +934,7 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -938,266 +953,266 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5"/>
+      <c r="F11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
`$column_definition->column_name` を `$column_definition->name` に名称変更。
</commit_message>
<xml_diff>
--- a/tests/testdata/db/sample_db_tables.xlsx
+++ b/tests/testdata/db/sample_db_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="table_user" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t xml:space="preserve">User Master Table</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">:columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">column_name</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
@@ -180,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Hiragino Mincho ProN"/>
@@ -201,55 +198,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Hiragino Mincho ProN"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -279,36 +227,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -318,44 +242,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -366,7 +263,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,61 +287,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,65 +301,49 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
@@ -522,7 +355,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -538,7 +371,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -567,20 +400,20 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.87"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3221153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3221153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7644230769231"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3221153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.54807692307692"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.4375"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.99519230769231"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3221153846154"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,43 +480,43 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>1</v>
@@ -698,10 +531,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
@@ -715,13 +548,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -733,13 +566,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -751,13 +584,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -767,13 +600,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -783,13 +616,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -801,13 +634,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -819,13 +652,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -837,13 +670,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -855,13 +688,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -874,7 +707,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -889,20 +722,20 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.87"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3221153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3221153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7644230769231"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3221153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.54807692307692"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.4375"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.99519230769231"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3221153846154"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,43 +800,43 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="7" t="n">
         <v>1</v>
@@ -1015,13 +848,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1032,18 +865,18 @@
         <v>1</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1055,13 +888,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1071,13 +904,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1089,13 +922,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1107,13 +940,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1125,13 +958,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1144,7 +977,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>